<commit_message>
Update data processing and visualization scripts
- Enhanced dataset creation with improved error handling and dataset existence checks
- Modified error flag analysis to use median metrics instead of mean
- Added detailed category-wise error analysis with comprehensive output
- Updated port selection mechanism for FiftyOne visualization
- Refined image processing and dataset loading functions
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_full_body_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_full_body_Filtered_Data_with_real_length.xlsx
@@ -751,7 +751,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a51c</t>
+          <t>67ceb73847361997ddc3c691</t>
         </is>
       </c>
       <c r="W2" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a51a</t>
+          <t>67ceb73847361997ddc3c68f</t>
         </is>
       </c>
       <c r="W3" t="n">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a51e</t>
+          <t>67ceb73847361997ddc3c693</t>
         </is>
       </c>
       <c r="W4" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>67cd3473ebee1dc3d760a368</t>
+          <t>67ceb73547361997ddc3c4dd</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>67cd3473ebee1dc3d760a36c</t>
+          <t>67ceb73547361997ddc3c4e1</t>
         </is>
       </c>
       <c r="W6" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>67cd3473ebee1dc3d760a36a</t>
+          <t>67ceb73547361997ddc3c4df</t>
         </is>
       </c>
       <c r="W7" t="n">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>67cd3473ebee1dc3d760a36e</t>
+          <t>67ceb73547361997ddc3c4e3</t>
         </is>
       </c>
       <c r="W8" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>67cd3484ebee1dc3d760a632</t>
+          <t>67ceb73947361997ddc3c7a7</t>
         </is>
       </c>
       <c r="W9" t="n">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>67cd3484ebee1dc3d760a634</t>
+          <t>67ceb73947361997ddc3c7a9</t>
         </is>
       </c>
       <c r="W10" t="n">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>67cd3484ebee1dc3d760a636</t>
+          <t>67ceb73947361997ddc3c7ab</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>67cd348cebee1dc3d760a784</t>
+          <t>67ceb73c47361997ddc3c8f9</t>
         </is>
       </c>
       <c r="W12" t="n">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>67cd348cebee1dc3d760a782</t>
+          <t>67ceb73c47361997ddc3c8f7</t>
         </is>
       </c>
       <c r="W13" t="n">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a4ed</t>
+          <t>67ceb73747361997ddc3c662</t>
         </is>
       </c>
       <c r="W14" t="n">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a4f1</t>
+          <t>67ceb73747361997ddc3c666</t>
         </is>
       </c>
       <c r="W15" t="n">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a4eb</t>
+          <t>67ceb73747361997ddc3c660</t>
         </is>
       </c>
       <c r="W16" t="n">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>67cd347debee1dc3d760a4ef</t>
+          <t>67ceb73747361997ddc3c664</t>
         </is>
       </c>
       <c r="W17" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>67cd3486ebee1dc3d760a68c</t>
+          <t>67ceb73a47361997ddc3c801</t>
         </is>
       </c>
       <c r="W18" t="n">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>67cd3486ebee1dc3d760a68e</t>
+          <t>67ceb73a47361997ddc3c803</t>
         </is>
       </c>
       <c r="W19" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>67cd3476ebee1dc3d760a3ea</t>
+          <t>67ceb73647361997ddc3c55f</t>
         </is>
       </c>
       <c r="W20" t="n">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>67cd3476ebee1dc3d760a3e8</t>
+          <t>67ceb73647361997ddc3c55d</t>
         </is>
       </c>
       <c r="W21" t="n">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>67cd3476ebee1dc3d760a3e6</t>
+          <t>67ceb73647361997ddc3c55b</t>
         </is>
       </c>
       <c r="W22" t="n">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>67cd346febee1dc3d760a318</t>
+          <t>67ceb73347361997ddc3c48d</t>
         </is>
       </c>
       <c r="W23" t="n">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>67cd346febee1dc3d760a31a</t>
+          <t>67ceb73347361997ddc3c48f</t>
         </is>
       </c>
       <c r="W24" t="n">
@@ -4431,7 +4431,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>67cd346febee1dc3d760a31c</t>
+          <t>67ceb73347361997ddc3c491</t>
         </is>
       </c>
       <c r="W25" t="n">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>67cd347bebee1dc3d760a4be</t>
+          <t>67ceb73747361997ddc3c633</t>
         </is>
       </c>
       <c r="W26" t="n">
@@ -4751,7 +4751,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>67cd347bebee1dc3d760a4bc</t>
+          <t>67ceb73747361997ddc3c631</t>
         </is>
       </c>
       <c r="W27" t="n">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>67cd347bebee1dc3d760a4c2</t>
+          <t>67ceb73747361997ddc3c637</t>
         </is>
       </c>
       <c r="W28" t="n">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>67cd3480ebee1dc3d760a578</t>
+          <t>67ceb73847361997ddc3c6ed</t>
         </is>
       </c>
       <c r="W29" t="n">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>67cd3480ebee1dc3d760a57c</t>
+          <t>67ceb73847361997ddc3c6f1</t>
         </is>
       </c>
       <c r="W30" t="n">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>67cd3480ebee1dc3d760a582</t>
+          <t>67ceb73847361997ddc3c6f7</t>
         </is>
       </c>
       <c r="W31" t="n">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>67cd3480ebee1dc3d760a57a</t>
+          <t>67ceb73847361997ddc3c6ef</t>
         </is>
       </c>
       <c r="W32" t="n">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>67cd3480ebee1dc3d760a57e</t>
+          <t>67ceb73847361997ddc3c6f3</t>
         </is>
       </c>
       <c r="W33" t="n">
@@ -5871,7 +5871,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>67cd3474ebee1dc3d760a3a8</t>
+          <t>67ceb73547361997ddc3c51d</t>
         </is>
       </c>
       <c r="W34" t="n">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>67cd3474ebee1dc3d760a3aa</t>
+          <t>67ceb73547361997ddc3c51f</t>
         </is>
       </c>
       <c r="W35" t="n">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>67cd3474ebee1dc3d760a3aa</t>
+          <t>67ceb73547361997ddc3c51f</t>
         </is>
       </c>
       <c r="W36" t="n">
@@ -6351,7 +6351,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>67cd347eebee1dc3d760a545</t>
+          <t>67ceb73847361997ddc3c6ba</t>
         </is>
       </c>
       <c r="W37" t="n">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>67cd347eebee1dc3d760a541</t>
+          <t>67ceb73847361997ddc3c6b6</t>
         </is>
       </c>
       <c r="W38" t="n">
@@ -6671,7 +6671,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>67cd347eebee1dc3d760a53d</t>
+          <t>67ceb73847361997ddc3c6b2</t>
         </is>
       </c>
       <c r="W39" t="n">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>67cd347eebee1dc3d760a53f</t>
+          <t>67ceb73847361997ddc3c6b4</t>
         </is>
       </c>
       <c r="W40" t="n">
@@ -6991,7 +6991,7 @@
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>67cd347eebee1dc3d760a543</t>
+          <t>67ceb73847361997ddc3c6b8</t>
         </is>
       </c>
       <c r="W41" t="n">
@@ -7151,7 +7151,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>67cd3485ebee1dc3d760a657</t>
+          <t>67ceb73a47361997ddc3c7cc</t>
         </is>
       </c>
       <c r="W42" t="n">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>67cd3485ebee1dc3d760a653</t>
+          <t>67ceb73a47361997ddc3c7c8</t>
         </is>
       </c>
       <c r="W43" t="n">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>67cd3485ebee1dc3d760a655</t>
+          <t>67ceb73a47361997ddc3c7ca</t>
         </is>
       </c>
       <c r="W44" t="n">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>67cd3485ebee1dc3d760a651</t>
+          <t>67ceb73a47361997ddc3c7c6</t>
         </is>
       </c>
       <c r="W45" t="n">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>67cd3482ebee1dc3d760a5c0</t>
+          <t>67ceb73947361997ddc3c735</t>
         </is>
       </c>
       <c r="W46" t="n">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>67cd3482ebee1dc3d760a5c2</t>
+          <t>67ceb73947361997ddc3c737</t>
         </is>
       </c>
       <c r="W47" t="n">
@@ -8111,7 +8111,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>67cd3482ebee1dc3d760a5c6</t>
+          <t>67ceb73947361997ddc3c73b</t>
         </is>
       </c>
       <c r="W48" t="n">
@@ -8271,7 +8271,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>67cd3482ebee1dc3d760a5c4</t>
+          <t>67ceb73947361997ddc3c739</t>
         </is>
       </c>
       <c r="W49" t="n">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>67cd3474ebee1dc3d760a393</t>
+          <t>67ceb73547361997ddc3c508</t>
         </is>
       </c>
       <c r="W50" t="n">
@@ -8591,7 +8591,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>67cd3474ebee1dc3d760a395</t>
+          <t>67ceb73547361997ddc3c50a</t>
         </is>
       </c>
       <c r="W51" t="n">
@@ -8751,7 +8751,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>67cd348cebee1dc3d760a797</t>
+          <t>67ceb73c47361997ddc3c90c</t>
         </is>
       </c>
       <c r="W52" t="n">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>67cd348cebee1dc3d760a799</t>
+          <t>67ceb73c47361997ddc3c90e</t>
         </is>
       </c>
       <c r="W53" t="n">
@@ -9071,7 +9071,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>67cd348cebee1dc3d760a79b</t>
+          <t>67ceb73c47361997ddc3c910</t>
         </is>
       </c>
       <c r="W54" t="n">
@@ -9231,7 +9231,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>67cd3483ebee1dc3d760a606</t>
+          <t>67ceb73947361997ddc3c77b</t>
         </is>
       </c>
       <c r="W55" t="n">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>67cd3483ebee1dc3d760a602</t>
+          <t>67ceb73947361997ddc3c777</t>
         </is>
       </c>
       <c r="W56" t="n">
@@ -9551,7 +9551,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>67cd3483ebee1dc3d760a600</t>
+          <t>67ceb73947361997ddc3c775</t>
         </is>
       </c>
       <c r="W57" t="n">
@@ -9711,7 +9711,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>67cd3488ebee1dc3d760a6e2</t>
+          <t>67ceb73a47361997ddc3c857</t>
         </is>
       </c>
       <c r="W58" t="n">
@@ -9871,7 +9871,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>67cd3488ebee1dc3d760a6e0</t>
+          <t>67ceb73a47361997ddc3c855</t>
         </is>
       </c>
       <c r="W59" t="n">
@@ -10031,7 +10031,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>67cd3488ebee1dc3d760a6e4</t>
+          <t>67ceb73a47361997ddc3c859</t>
         </is>
       </c>
       <c r="W60" t="n">
@@ -10191,7 +10191,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>67cd3488ebee1dc3d760a6e6</t>
+          <t>67ceb73a47361997ddc3c85b</t>
         </is>
       </c>
       <c r="W61" t="n">
@@ -10351,7 +10351,7 @@
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>67cd3478ebee1dc3d760a434</t>
+          <t>67ceb73647361997ddc3c5a9</t>
         </is>
       </c>
       <c r="W62" t="n">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>67cd3478ebee1dc3d760a436</t>
+          <t>67ceb73647361997ddc3c5ab</t>
         </is>
       </c>
       <c r="W63" t="n">
@@ -10671,7 +10671,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>67cd3478ebee1dc3d760a432</t>
+          <t>67ceb73647361997ddc3c5a7</t>
         </is>
       </c>
       <c r="W64" t="n">
@@ -10831,7 +10831,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>67cd3479ebee1dc3d760a46e</t>
+          <t>67ceb73747361997ddc3c5e3</t>
         </is>
       </c>
       <c r="W65" t="n">
@@ -10991,7 +10991,7 @@
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>67cd3479ebee1dc3d760a472</t>
+          <t>67ceb73747361997ddc3c5e7</t>
         </is>
       </c>
       <c r="W66" t="n">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>67cd3479ebee1dc3d760a457</t>
+          <t>67ceb73647361997ddc3c5cc</t>
         </is>
       </c>
       <c r="W67" t="n">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>67cd3479ebee1dc3d760a455</t>
+          <t>67ceb73647361997ddc3c5ca</t>
         </is>
       </c>
       <c r="W68" t="n">
@@ -11471,7 +11471,7 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>67cd3489ebee1dc3d760a71b</t>
+          <t>67ceb73b47361997ddc3c890</t>
         </is>
       </c>
       <c r="W69" t="n">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>67cd3489ebee1dc3d760a717</t>
+          <t>67ceb73b47361997ddc3c88c</t>
         </is>
       </c>
       <c r="W70" t="n">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>67cd3489ebee1dc3d760a713</t>
+          <t>67ceb73b47361997ddc3c888</t>
         </is>
       </c>
       <c r="W71" t="n">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>67cd347aebee1dc3d760a48f</t>
+          <t>67ceb73747361997ddc3c604</t>
         </is>
       </c>
       <c r="W72" t="n">
@@ -12111,7 +12111,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>67cd347aebee1dc3d760a48b</t>
+          <t>67ceb73747361997ddc3c600</t>
         </is>
       </c>
       <c r="W73" t="n">
@@ -12271,7 +12271,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>67cd347aebee1dc3d760a491</t>
+          <t>67ceb73747361997ddc3c606</t>
         </is>
       </c>
       <c r="W74" t="n">
@@ -12431,7 +12431,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>67cd347aebee1dc3d760a48d</t>
+          <t>67ceb73747361997ddc3c602</t>
         </is>
       </c>
       <c r="W75" t="n">
@@ -12591,7 +12591,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>67cd3490ebee1dc3d760a80b</t>
+          <t>67ceb73d47361997ddc3c980</t>
         </is>
       </c>
       <c r="W76" t="n">
@@ -12751,7 +12751,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>67cd3490ebee1dc3d760a80f</t>
+          <t>67ceb73d47361997ddc3c984</t>
         </is>
       </c>
       <c r="W77" t="n">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>67cd3490ebee1dc3d760a80d</t>
+          <t>67ceb73d47361997ddc3c982</t>
         </is>
       </c>
       <c r="W78" t="n">
@@ -13071,7 +13071,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>67cd3490ebee1dc3d760a811</t>
+          <t>67ceb73d47361997ddc3c986</t>
         </is>
       </c>
       <c r="W79" t="n">
@@ -13231,7 +13231,7 @@
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>67cd3477ebee1dc3d760a41a</t>
+          <t>67ceb73647361997ddc3c58f</t>
         </is>
       </c>
       <c r="W80" t="n">
@@ -13391,7 +13391,7 @@
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>67cd3491ebee1dc3d760a838</t>
+          <t>67ceb73d47361997ddc3c9ad</t>
         </is>
       </c>
       <c r="W81" t="n">
@@ -13551,7 +13551,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>67cd3491ebee1dc3d760a836</t>
+          <t>67ceb73d47361997ddc3c9ab</t>
         </is>
       </c>
       <c r="W82" t="n">
@@ -13711,7 +13711,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>67cd3491ebee1dc3d760a83a</t>
+          <t>67ceb73d47361997ddc3c9af</t>
         </is>
       </c>
       <c r="W83" t="n">
@@ -13871,7 +13871,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>67cd3487ebee1dc3d760a6a5</t>
+          <t>67ceb73a47361997ddc3c81a</t>
         </is>
       </c>
       <c r="W84" t="n">
@@ -14031,7 +14031,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>67cd3487ebee1dc3d760a6a7</t>
+          <t>67ceb73a47361997ddc3c81c</t>
         </is>
       </c>
       <c r="W85" t="n">
@@ -14191,7 +14191,7 @@
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>67cd3487ebee1dc3d760a6be</t>
+          <t>67ceb73a47361997ddc3c833</t>
         </is>
       </c>
       <c r="W86" t="n">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>67cd348debee1dc3d760a7b6</t>
+          <t>67ceb73c47361997ddc3c92b</t>
         </is>
       </c>
       <c r="W87" t="n">
@@ -14511,7 +14511,7 @@
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>67cd3488ebee1dc3d760a6d5</t>
+          <t>67ceb73a47361997ddc3c84a</t>
         </is>
       </c>
       <c r="W88" t="n">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>67cd3475ebee1dc3d760a3cd</t>
+          <t>67ceb73647361997ddc3c542</t>
         </is>
       </c>
       <c r="W89" t="n">
@@ -14831,7 +14831,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>67cd3475ebee1dc3d760a3cb</t>
+          <t>67ceb73647361997ddc3c540</t>
         </is>
       </c>
       <c r="W90" t="n">
@@ -14991,7 +14991,7 @@
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>67cd3472ebee1dc3d760a33f</t>
+          <t>67ceb73447361997ddc3c4b4</t>
         </is>
       </c>
       <c r="W91" t="n">
@@ -15151,7 +15151,7 @@
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>67cd3472ebee1dc3d760a341</t>
+          <t>67ceb73447361997ddc3c4b6</t>
         </is>
       </c>
       <c r="W92" t="n">
@@ -15311,7 +15311,7 @@
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>67cd3472ebee1dc3d760a33b</t>
+          <t>67ceb73447361997ddc3c4b0</t>
         </is>
       </c>
       <c r="W93" t="n">
@@ -15471,7 +15471,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>67cd3472ebee1dc3d760a33d</t>
+          <t>67ceb73447361997ddc3c4b2</t>
         </is>
       </c>
       <c r="W94" t="n">
@@ -15631,7 +15631,7 @@
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>67cd348bebee1dc3d760a753</t>
+          <t>67ceb73b47361997ddc3c8c8</t>
         </is>
       </c>
       <c r="W95" t="n">
@@ -15791,7 +15791,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>67cd348bebee1dc3d760a755</t>
+          <t>67ceb73b47361997ddc3c8ca</t>
         </is>
       </c>
       <c r="W96" t="n">
@@ -15951,7 +15951,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>67cd348bebee1dc3d760a759</t>
+          <t>67ceb73b47361997ddc3c8ce</t>
         </is>
       </c>
       <c r="W97" t="n">
@@ -16111,7 +16111,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>67cd348bebee1dc3d760a757</t>
+          <t>67ceb73b47361997ddc3c8cc</t>
         </is>
       </c>
       <c r="W98" t="n">
@@ -16271,7 +16271,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>67cd348aebee1dc3d760a740</t>
+          <t>67ceb73b47361997ddc3c8b5</t>
         </is>
       </c>
       <c r="W99" t="n">
@@ -16431,7 +16431,7 @@
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>67cd348aebee1dc3d760a73e</t>
+          <t>67ceb73b47361997ddc3c8b3</t>
         </is>
       </c>
       <c r="W100" t="n">
@@ -16591,7 +16591,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>67cd3484ebee1dc3d760a621</t>
+          <t>67ceb73947361997ddc3c796</t>
         </is>
       </c>
       <c r="W101" t="n">
@@ -16751,7 +16751,7 @@
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>67cd348febee1dc3d760a7d6</t>
+          <t>67ceb73c47361997ddc3c94b</t>
         </is>
       </c>
       <c r="W102" t="n">
@@ -16911,7 +16911,7 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>67cd348febee1dc3d760a7de</t>
+          <t>67ceb73c47361997ddc3c953</t>
         </is>
       </c>
       <c r="W103" t="n">
@@ -17071,7 +17071,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>67cd348febee1dc3d760a7de</t>
+          <t>67ceb73c47361997ddc3c953</t>
         </is>
       </c>
       <c r="W104" t="n">
@@ -17231,7 +17231,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>67cd348febee1dc3d760a7d8</t>
+          <t>67ceb73c47361997ddc3c94d</t>
         </is>
       </c>
       <c r="W105" t="n">
@@ -17391,7 +17391,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>67cd348febee1dc3d760a7da</t>
+          <t>67ceb73c47361997ddc3c94f</t>
         </is>
       </c>
       <c r="W106" t="n">
@@ -17551,7 +17551,7 @@
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>67cd348eebee1dc3d760a7c5</t>
+          <t>67ceb73c47361997ddc3c93a</t>
         </is>
       </c>
       <c r="W107" t="n">
@@ -17711,7 +17711,7 @@
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>67cd3492ebee1dc3d760a863</t>
+          <t>67ceb73d47361997ddc3c9d8</t>
         </is>
       </c>
       <c r="W108" t="n">
@@ -17871,7 +17871,7 @@
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>67cd3492ebee1dc3d760a861</t>
+          <t>67ceb73d47361997ddc3c9d6</t>
         </is>
       </c>
       <c r="W109" t="n">
@@ -18031,7 +18031,7 @@
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>67cd3494ebee1dc3d760a8aa</t>
+          <t>67ceb73e47361997ddc3ca1f</t>
         </is>
       </c>
       <c r="W110" t="n">
@@ -18191,7 +18191,7 @@
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>67cd3494ebee1dc3d760a8ae</t>
+          <t>67ceb73e47361997ddc3ca23</t>
         </is>
       </c>
       <c r="W111" t="n">
@@ -18447,7 +18447,7 @@
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>67cd3499ebee1dc3d760a98c</t>
+          <t>67ceb73f47361997ddc3cb01</t>
         </is>
       </c>
       <c r="W113" t="n">
@@ -18703,7 +18703,7 @@
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>67cd3495ebee1dc3d760a8c3</t>
+          <t>67ceb73e47361997ddc3ca38</t>
         </is>
       </c>
       <c r="W115" t="n">
@@ -18863,7 +18863,7 @@
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>67cd3496ebee1dc3d760a923</t>
+          <t>67ceb73f47361997ddc3ca98</t>
         </is>
       </c>
       <c r="W116" t="n">
@@ -19407,7 +19407,7 @@
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>67cd3497ebee1dc3d760a940</t>
+          <t>67ceb73f47361997ddc3cab5</t>
         </is>
       </c>
       <c r="W121" t="n">
@@ -19567,7 +19567,7 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>67cd3496ebee1dc3d760a92e</t>
+          <t>67ceb73f47361997ddc3caa3</t>
         </is>
       </c>
       <c r="W122" t="n">
@@ -20111,7 +20111,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>67cd3497ebee1dc3d760a950</t>
+          <t>67ceb73f47361997ddc3cac5</t>
         </is>
       </c>
       <c r="W127" t="n">
@@ -20271,7 +20271,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>67cd3495ebee1dc3d760a8e5</t>
+          <t>67ceb73e47361997ddc3ca5a</t>
         </is>
       </c>
       <c r="W128" t="n">
@@ -20431,7 +20431,7 @@
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>67cd3498ebee1dc3d760a962</t>
+          <t>67ceb73f47361997ddc3cad7</t>
         </is>
       </c>
       <c r="W129" t="n">
@@ -20591,7 +20591,7 @@
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>67cd3498ebee1dc3d760a96f</t>
+          <t>67ceb73f47361997ddc3cae4</t>
         </is>
       </c>
       <c r="W130" t="n">
@@ -20751,7 +20751,7 @@
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>67cd3494ebee1dc3d760a895</t>
+          <t>67ceb73e47361997ddc3ca0a</t>
         </is>
       </c>
       <c r="W131" t="n">
@@ -20911,7 +20911,7 @@
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>67cd3498ebee1dc3d760a97f</t>
+          <t>67ceb73f47361997ddc3caf4</t>
         </is>
       </c>
       <c r="W132" t="n">
@@ -21071,7 +21071,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>67cd3496ebee1dc3d760a90b</t>
+          <t>67ceb73f47361997ddc3ca80</t>
         </is>
       </c>
       <c r="W133" t="n">

</xml_diff>

<commit_message>
create fiftyone dataset of molt
</commit_message>
<xml_diff>
--- a/fifty_one/measurements/Updated_full_body_Filtered_Data_with_real_length.xlsx
+++ b/fifty_one/measurements/Updated_full_body_Filtered_Data_with_real_length.xlsx
@@ -751,7 +751,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bd3</t>
+          <t>67e72c4acde4e894925703ff</t>
         </is>
       </c>
       <c r="W2" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bd1</t>
+          <t>67e72c4acde4e894925703fd</t>
         </is>
       </c>
       <c r="W3" t="n">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bd5</t>
+          <t>67e72c4acde4e89492570401</t>
         </is>
       </c>
       <c r="W4" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a1f</t>
+          <t>67e72c49cde4e8949257024b</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a23</t>
+          <t>67e72c49cde4e8949257024f</t>
         </is>
       </c>
       <c r="W6" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a21</t>
+          <t>67e72c49cde4e8949257024d</t>
         </is>
       </c>
       <c r="W7" t="n">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a25</t>
+          <t>67e72c49cde4e89492570251</t>
         </is>
       </c>
       <c r="W8" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ce9</t>
+          <t>67e72c4acde4e89492570515</t>
         </is>
       </c>
       <c r="W9" t="n">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ceb</t>
+          <t>67e72c4acde4e89492570517</t>
         </is>
       </c>
       <c r="W10" t="n">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ced</t>
+          <t>67e72c4acde4e89492570519</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e3b</t>
+          <t>67e72c4acde4e89492570667</t>
         </is>
       </c>
       <c r="W12" t="n">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e39</t>
+          <t>67e72c4acde4e89492570665</t>
         </is>
       </c>
       <c r="W13" t="n">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356ba4</t>
+          <t>67e72c49cde4e894925703d0</t>
         </is>
       </c>
       <c r="W14" t="n">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356ba8</t>
+          <t>67e72c49cde4e894925703d4</t>
         </is>
       </c>
       <c r="W15" t="n">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356ba2</t>
+          <t>67e72c49cde4e894925703ce</t>
         </is>
       </c>
       <c r="W16" t="n">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356ba6</t>
+          <t>67e72c49cde4e894925703d2</t>
         </is>
       </c>
       <c r="W17" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d43</t>
+          <t>67e72c4acde4e8949257056f</t>
         </is>
       </c>
       <c r="W18" t="n">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d45</t>
+          <t>67e72c4acde4e89492570571</t>
         </is>
       </c>
       <c r="W19" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356aa1</t>
+          <t>67e72c49cde4e894925702cd</t>
         </is>
       </c>
       <c r="W20" t="n">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a9f</t>
+          <t>67e72c49cde4e894925702cb</t>
         </is>
       </c>
       <c r="W21" t="n">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a9d</t>
+          <t>67e72c49cde4e894925702c9</t>
         </is>
       </c>
       <c r="W22" t="n">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569cf</t>
+          <t>67e72c48cde4e894925701fb</t>
         </is>
       </c>
       <c r="W23" t="n">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569d1</t>
+          <t>67e72c48cde4e894925701fd</t>
         </is>
       </c>
       <c r="W24" t="n">
@@ -4431,7 +4431,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569d3</t>
+          <t>67e72c48cde4e894925701ff</t>
         </is>
       </c>
       <c r="W25" t="n">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b75</t>
+          <t>67e72c49cde4e894925703a1</t>
         </is>
       </c>
       <c r="W26" t="n">
@@ -4751,7 +4751,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b73</t>
+          <t>67e72c49cde4e8949257039f</t>
         </is>
       </c>
       <c r="W27" t="n">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b79</t>
+          <t>67e72c49cde4e894925703a5</t>
         </is>
       </c>
       <c r="W28" t="n">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c2f</t>
+          <t>67e72c4acde4e8949257045b</t>
         </is>
       </c>
       <c r="W29" t="n">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c33</t>
+          <t>67e72c4acde4e8949257045f</t>
         </is>
       </c>
       <c r="W30" t="n">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c39</t>
+          <t>67e72c4acde4e89492570465</t>
         </is>
       </c>
       <c r="W31" t="n">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c31</t>
+          <t>67e72c4acde4e8949257045d</t>
         </is>
       </c>
       <c r="W32" t="n">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c35</t>
+          <t>67e72c4acde4e89492570461</t>
         </is>
       </c>
       <c r="W33" t="n">
@@ -5871,7 +5871,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a5f</t>
+          <t>67e72c49cde4e8949257028b</t>
         </is>
       </c>
       <c r="W34" t="n">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a61</t>
+          <t>67e72c49cde4e8949257028d</t>
         </is>
       </c>
       <c r="W35" t="n">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a61</t>
+          <t>67e72c49cde4e8949257028d</t>
         </is>
       </c>
       <c r="W36" t="n">
@@ -6351,7 +6351,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bfc</t>
+          <t>67e72c4acde4e89492570428</t>
         </is>
       </c>
       <c r="W37" t="n">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bf8</t>
+          <t>67e72c4acde4e89492570424</t>
         </is>
       </c>
       <c r="W38" t="n">
@@ -6671,7 +6671,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bf4</t>
+          <t>67e72c4acde4e89492570420</t>
         </is>
       </c>
       <c r="W39" t="n">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bf6</t>
+          <t>67e72c4acde4e89492570422</t>
         </is>
       </c>
       <c r="W40" t="n">
@@ -6991,7 +6991,7 @@
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356bfa</t>
+          <t>67e72c4acde4e89492570426</t>
         </is>
       </c>
       <c r="W41" t="n">
@@ -7151,7 +7151,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d0e</t>
+          <t>67e72c4acde4e8949257053a</t>
         </is>
       </c>
       <c r="W42" t="n">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d0a</t>
+          <t>67e72c4acde4e89492570536</t>
         </is>
       </c>
       <c r="W43" t="n">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d0c</t>
+          <t>67e72c4acde4e89492570538</t>
         </is>
       </c>
       <c r="W44" t="n">
@@ -7631,7 +7631,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d08</t>
+          <t>67e72c4acde4e89492570534</t>
         </is>
       </c>
       <c r="W45" t="n">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c77</t>
+          <t>67e72c4acde4e894925704a3</t>
         </is>
       </c>
       <c r="W46" t="n">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c79</t>
+          <t>67e72c4acde4e894925704a5</t>
         </is>
       </c>
       <c r="W47" t="n">
@@ -8111,7 +8111,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c7d</t>
+          <t>67e72c4acde4e894925704a9</t>
         </is>
       </c>
       <c r="W48" t="n">
@@ -8271,7 +8271,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356c7b</t>
+          <t>67e72c4acde4e894925704a7</t>
         </is>
       </c>
       <c r="W49" t="n">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a4a</t>
+          <t>67e72c49cde4e89492570276</t>
         </is>
       </c>
       <c r="W50" t="n">
@@ -8591,7 +8591,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a4c</t>
+          <t>67e72c49cde4e89492570278</t>
         </is>
       </c>
       <c r="W51" t="n">
@@ -8751,7 +8751,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e4e</t>
+          <t>67e72c4acde4e8949257067a</t>
         </is>
       </c>
       <c r="W52" t="n">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e50</t>
+          <t>67e72c4acde4e8949257067c</t>
         </is>
       </c>
       <c r="W53" t="n">
@@ -9071,7 +9071,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e52</t>
+          <t>67e72c4acde4e8949257067e</t>
         </is>
       </c>
       <c r="W54" t="n">
@@ -9231,7 +9231,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356cbd</t>
+          <t>67e72c4acde4e894925704e9</t>
         </is>
       </c>
       <c r="W55" t="n">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356cb9</t>
+          <t>67e72c4acde4e894925704e5</t>
         </is>
       </c>
       <c r="W56" t="n">
@@ -9551,7 +9551,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356cb7</t>
+          <t>67e72c4acde4e894925704e3</t>
         </is>
       </c>
       <c r="W57" t="n">
@@ -9711,7 +9711,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d99</t>
+          <t>67e72c4acde4e894925705c5</t>
         </is>
       </c>
       <c r="W58" t="n">
@@ -9871,7 +9871,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d97</t>
+          <t>67e72c4acde4e894925705c3</t>
         </is>
       </c>
       <c r="W59" t="n">
@@ -10031,7 +10031,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d9b</t>
+          <t>67e72c4acde4e894925705c7</t>
         </is>
       </c>
       <c r="W60" t="n">
@@ -10191,7 +10191,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d9d</t>
+          <t>67e72c4acde4e894925705c9</t>
         </is>
       </c>
       <c r="W61" t="n">
@@ -10351,7 +10351,7 @@
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356aeb</t>
+          <t>67e72c49cde4e89492570317</t>
         </is>
       </c>
       <c r="W62" t="n">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356aed</t>
+          <t>67e72c49cde4e89492570319</t>
         </is>
       </c>
       <c r="W63" t="n">
@@ -10671,7 +10671,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356ae9</t>
+          <t>67e72c49cde4e89492570315</t>
         </is>
       </c>
       <c r="W64" t="n">
@@ -10831,7 +10831,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b25</t>
+          <t>67e72c49cde4e89492570351</t>
         </is>
       </c>
       <c r="W65" t="n">
@@ -10991,7 +10991,7 @@
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b29</t>
+          <t>67e72c49cde4e89492570355</t>
         </is>
       </c>
       <c r="W66" t="n">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b0e</t>
+          <t>67e72c49cde4e8949257033a</t>
         </is>
       </c>
       <c r="W67" t="n">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b0c</t>
+          <t>67e72c49cde4e89492570338</t>
         </is>
       </c>
       <c r="W68" t="n">
@@ -11471,7 +11471,7 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356dd2</t>
+          <t>67e72c4acde4e894925705fe</t>
         </is>
       </c>
       <c r="W69" t="n">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356dce</t>
+          <t>67e72c4acde4e894925705fa</t>
         </is>
       </c>
       <c r="W70" t="n">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356dca</t>
+          <t>67e72c4acde4e894925705f6</t>
         </is>
       </c>
       <c r="W71" t="n">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b46</t>
+          <t>67e72c49cde4e89492570372</t>
         </is>
       </c>
       <c r="W72" t="n">
@@ -12111,7 +12111,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b42</t>
+          <t>67e72c49cde4e8949257036e</t>
         </is>
       </c>
       <c r="W73" t="n">
@@ -12271,7 +12271,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b48</t>
+          <t>67e72c49cde4e89492570374</t>
         </is>
       </c>
       <c r="W74" t="n">
@@ -12431,7 +12431,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356b44</t>
+          <t>67e72c49cde4e89492570370</t>
         </is>
       </c>
       <c r="W75" t="n">
@@ -12591,7 +12591,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ec2</t>
+          <t>67e72c4bcde4e894925706ee</t>
         </is>
       </c>
       <c r="W76" t="n">
@@ -12751,7 +12751,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ec6</t>
+          <t>67e72c4bcde4e894925706f2</t>
         </is>
       </c>
       <c r="W77" t="n">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ec4</t>
+          <t>67e72c4bcde4e894925706f0</t>
         </is>
       </c>
       <c r="W78" t="n">
@@ -13071,7 +13071,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356ec8</t>
+          <t>67e72c4bcde4e894925706f4</t>
         </is>
       </c>
       <c r="W79" t="n">
@@ -13231,7 +13231,7 @@
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356ad1</t>
+          <t>67e72c49cde4e894925702fd</t>
         </is>
       </c>
       <c r="W80" t="n">
@@ -13391,7 +13391,7 @@
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356eef</t>
+          <t>67e72c4bcde4e8949257071b</t>
         </is>
       </c>
       <c r="W81" t="n">
@@ -13551,7 +13551,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356eed</t>
+          <t>67e72c4bcde4e89492570719</t>
         </is>
       </c>
       <c r="W82" t="n">
@@ -13711,7 +13711,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356ef1</t>
+          <t>67e72c4bcde4e8949257071d</t>
         </is>
       </c>
       <c r="W83" t="n">
@@ -13871,7 +13871,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d5c</t>
+          <t>67e72c4acde4e89492570588</t>
         </is>
       </c>
       <c r="W84" t="n">
@@ -14031,7 +14031,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d5e</t>
+          <t>67e72c4acde4e8949257058a</t>
         </is>
       </c>
       <c r="W85" t="n">
@@ -14191,7 +14191,7 @@
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d75</t>
+          <t>67e72c4acde4e894925705a1</t>
         </is>
       </c>
       <c r="W86" t="n">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e6d</t>
+          <t>67e72c4acde4e89492570699</t>
         </is>
       </c>
       <c r="W87" t="n">
@@ -14511,7 +14511,7 @@
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356d8c</t>
+          <t>67e72c4acde4e894925705b8</t>
         </is>
       </c>
       <c r="W88" t="n">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a84</t>
+          <t>67e72c49cde4e894925702b0</t>
         </is>
       </c>
       <c r="W89" t="n">
@@ -14831,7 +14831,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>67e036b8454164a56f356a82</t>
+          <t>67e72c49cde4e894925702ae</t>
         </is>
       </c>
       <c r="W90" t="n">
@@ -14991,7 +14991,7 @@
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569f6</t>
+          <t>67e72c49cde4e89492570222</t>
         </is>
       </c>
       <c r="W91" t="n">
@@ -15151,7 +15151,7 @@
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569f8</t>
+          <t>67e72c49cde4e89492570224</t>
         </is>
       </c>
       <c r="W92" t="n">
@@ -15311,7 +15311,7 @@
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569f2</t>
+          <t>67e72c49cde4e8949257021e</t>
         </is>
       </c>
       <c r="W93" t="n">
@@ -15471,7 +15471,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>67e036b7454164a56f3569f4</t>
+          <t>67e72c49cde4e89492570220</t>
         </is>
       </c>
       <c r="W94" t="n">
@@ -15631,7 +15631,7 @@
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e0a</t>
+          <t>67e72c4acde4e89492570636</t>
         </is>
       </c>
       <c r="W95" t="n">
@@ -15791,7 +15791,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e0c</t>
+          <t>67e72c4acde4e89492570638</t>
         </is>
       </c>
       <c r="W96" t="n">
@@ -15951,7 +15951,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e10</t>
+          <t>67e72c4acde4e8949257063c</t>
         </is>
       </c>
       <c r="W97" t="n">
@@ -16111,7 +16111,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e0e</t>
+          <t>67e72c4acde4e8949257063a</t>
         </is>
       </c>
       <c r="W98" t="n">
@@ -16271,7 +16271,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356df7</t>
+          <t>67e72c4acde4e89492570623</t>
         </is>
       </c>
       <c r="W99" t="n">
@@ -16431,7 +16431,7 @@
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356df5</t>
+          <t>67e72c4acde4e89492570621</t>
         </is>
       </c>
       <c r="W100" t="n">
@@ -16591,7 +16591,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356cd8</t>
+          <t>67e72c4acde4e89492570504</t>
         </is>
       </c>
       <c r="W101" t="n">
@@ -16751,7 +16751,7 @@
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e8d</t>
+          <t>67e72c4bcde4e894925706b9</t>
         </is>
       </c>
       <c r="W102" t="n">
@@ -16911,7 +16911,7 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e95</t>
+          <t>67e72c4bcde4e894925706c1</t>
         </is>
       </c>
       <c r="W103" t="n">
@@ -17071,7 +17071,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e95</t>
+          <t>67e72c4bcde4e894925706c1</t>
         </is>
       </c>
       <c r="W104" t="n">
@@ -17231,7 +17231,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e8f</t>
+          <t>67e72c4bcde4e894925706bb</t>
         </is>
       </c>
       <c r="W105" t="n">
@@ -17391,7 +17391,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e91</t>
+          <t>67e72c4bcde4e894925706bd</t>
         </is>
       </c>
       <c r="W106" t="n">
@@ -17551,7 +17551,7 @@
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>67e036b9454164a56f356e7c</t>
+          <t>67e72c4bcde4e894925706a8</t>
         </is>
       </c>
       <c r="W107" t="n">
@@ -17711,7 +17711,7 @@
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f1a</t>
+          <t>67e72c4bcde4e89492570746</t>
         </is>
       </c>
       <c r="W108" t="n">
@@ -17871,7 +17871,7 @@
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f18</t>
+          <t>67e72c4bcde4e89492570744</t>
         </is>
       </c>
       <c r="W109" t="n">
@@ -18031,7 +18031,7 @@
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f61</t>
+          <t>67e72c4bcde4e8949257078d</t>
         </is>
       </c>
       <c r="W110" t="n">
@@ -18191,7 +18191,7 @@
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f65</t>
+          <t>67e72c4bcde4e89492570791</t>
         </is>
       </c>
       <c r="W111" t="n">
@@ -18447,7 +18447,7 @@
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f357043</t>
+          <t>67e72c4bcde4e8949257086f</t>
         </is>
       </c>
       <c r="W113" t="n">
@@ -18703,7 +18703,7 @@
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f7a</t>
+          <t>67e72c4bcde4e894925707a6</t>
         </is>
       </c>
       <c r="W115" t="n">
@@ -18863,7 +18863,7 @@
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356fda</t>
+          <t>67e72c4bcde4e89492570806</t>
         </is>
       </c>
       <c r="W116" t="n">
@@ -19407,7 +19407,7 @@
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356ff7</t>
+          <t>67e72c4bcde4e89492570823</t>
         </is>
       </c>
       <c r="W121" t="n">
@@ -19567,7 +19567,7 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356fe5</t>
+          <t>67e72c4bcde4e89492570811</t>
         </is>
       </c>
       <c r="W122" t="n">
@@ -20111,7 +20111,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f357007</t>
+          <t>67e72c4bcde4e89492570833</t>
         </is>
       </c>
       <c r="W127" t="n">
@@ -20271,7 +20271,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f9c</t>
+          <t>67e72c4bcde4e894925707c8</t>
         </is>
       </c>
       <c r="W128" t="n">
@@ -20431,7 +20431,7 @@
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f357019</t>
+          <t>67e72c4bcde4e89492570845</t>
         </is>
       </c>
       <c r="W129" t="n">
@@ -20591,7 +20591,7 @@
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f357026</t>
+          <t>67e72c4bcde4e89492570852</t>
         </is>
       </c>
       <c r="W130" t="n">
@@ -20751,7 +20751,7 @@
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356f4c</t>
+          <t>67e72c4bcde4e89492570778</t>
         </is>
       </c>
       <c r="W131" t="n">
@@ -20911,7 +20911,7 @@
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f357036</t>
+          <t>67e72c4bcde4e89492570862</t>
         </is>
       </c>
       <c r="W132" t="n">
@@ -21071,7 +21071,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>67e036ba454164a56f356fc2</t>
+          <t>67e72c4bcde4e894925707ee</t>
         </is>
       </c>
       <c r="W133" t="n">

</xml_diff>